<commit_message>
new colums, new filters, change dates by season feature, search box choices fixed
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Scientific Name</t>
   </si>
@@ -26,42 +26,6 @@
   </si>
   <si>
     <t>Relative Frequency %</t>
-  </si>
-  <si>
-    <t>Xenoglaux loweryi</t>
-  </si>
-  <si>
-    <t>Long-whiskered Owlet</t>
-  </si>
-  <si>
-    <t>33.33</t>
-  </si>
-  <si>
-    <t>Drymophila striaticeps</t>
-  </si>
-  <si>
-    <t>Streak-headed Antbird</t>
-  </si>
-  <si>
-    <t>16.67</t>
-  </si>
-  <si>
-    <t>Grallaricula ochraceifrons</t>
-  </si>
-  <si>
-    <t>Ochre-fronted Antpitta</t>
-  </si>
-  <si>
-    <t>Pseudotriccus ruficeps</t>
-  </si>
-  <si>
-    <t>Rufous-headed Pygmy-Tyrant</t>
-  </si>
-  <si>
-    <t>Poecilotriccus luluae</t>
-  </si>
-  <si>
-    <t>Johnson's Tody-Flycatcher</t>
   </si>
 </sst>
 </file>
@@ -396,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -416,76 +380,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
+    <row r="2" spans="1:4" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>